<commit_message>
Adding modules for real-time LPF control, fixed Butterworth filter
</commit_message>
<xml_diff>
--- a/Matlab/DSPfilterFunctions/RealTimeLPFs/filter_summary.xlsx
+++ b/Matlab/DSPfilterFunctions/RealTimeLPFs/filter_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\Desktop\covg_fpga\Matlab\DSPfilterFunctions\RealTimeLPFs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A906FA-A7EE-489E-982E-2AD8E8F191A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0519CB-C596-4013-9049-3F943376338B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67E4EFBA-62CC-CB43-BD72-BACC4EAC0B39}"/>
   </bookViews>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="42">
   <si>
     <t>Filter name</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>Not yet tested</t>
+  </si>
+  <si>
+    <t>250 kHz</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -917,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB5AD64-B730-394B-9445-B2A0CBB59F5E}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L2" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1056,13 +1055,13 @@
         <v>14</v>
       </c>
       <c r="G5">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J5">
         <v>4</v>

</xml_diff>